<commit_message>
tabela do summary gotowa
</commit_message>
<xml_diff>
--- a/src/assets/kr2018.xlsx
+++ b/src/assets/kr2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lista braci - Reg. 2018" sheetId="1" state="visible" r:id="rId2"/>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">mężczyzna chory</t>
   </si>
   <si>
-    <t xml:space="preserve">razem na salę gimn. (krzesła - z nianiami i dziećmi) </t>
+    <t xml:space="preserve">razem na salę gimn. (krzesła - z nianiami i dziećmi)</t>
   </si>
   <si>
     <t xml:space="preserve">3-os. z dzieckiem (ew. z nianią rodzinną)</t>
@@ -6006,8 +6006,8 @@
   </sheetPr>
   <dimension ref="A1:Y1540"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A339" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="W9" s="14"/>
     </row>
-    <row r="10" s="12" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="59"/>
       <c r="B10" s="60"/>
       <c r="C10" s="70"/>
@@ -34170,7 +34170,7 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A148" activeCellId="0" sqref="A148"/>
     </sheetView>
   </sheetViews>
@@ -38445,7 +38445,7 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A171" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A176" activeCellId="0" sqref="A176"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding new participant to the store..
</commit_message>
<xml_diff>
--- a/src/assets/kr2018.xlsx
+++ b/src/assets/kr2018.xlsx
@@ -2652,9 +2652,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="19" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="19" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -6006,7 +6006,7 @@
   </sheetPr>
   <dimension ref="A1:Y1540"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A514" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -6273,7 +6273,7 @@
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
     </row>
-    <row r="7" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="59"/>
       <c r="B7" s="60" t="str">
         <f aca="false">B1</f>

</xml_diff>